<commit_message>
Slight Fix to Lab 5
</commit_message>
<xml_diff>
--- a/Lab 5/control_store_lab_5.xlsx
+++ b/Lab 5/control_store_lab_5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ffacd89b2f1a651/Documents/Current Classes/ECE 460N/Labs/Lab 5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1636" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CD3B660-F374-456B-B227-F1E74116EAE7}"/>
+  <xr:revisionPtr revIDLastSave="1667" documentId="8_{E8B15512-F0F0-402B-966B-8983E744E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{726EB0EE-D177-4839-9573-25EE57DE3F70}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4209" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4339" uniqueCount="117">
   <si>
     <t>000000  (state 0)</t>
   </si>
@@ -366,6 +366,12 @@
   <si>
     <t>RETSTATE</t>
   </si>
+  <si>
+    <t>LD.SMDR</t>
+  </si>
+  <si>
+    <t>MDRMUX</t>
+  </si>
 </sst>
 </file>
 
@@ -632,6 +638,11 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -641,11 +652,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,6 +667,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -960,11 +970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN65"/>
+  <dimension ref="A1:BO65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S78" sqref="S78"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -980,11 +990,11 @@
     <col min="20" max="42" width="2.453125" style="1" customWidth="1"/>
     <col min="43" max="56" width="2.453125" style="3" customWidth="1"/>
     <col min="57" max="58" width="2.453125" style="1" customWidth="1"/>
-    <col min="59" max="66" width="2.453125" style="3" customWidth="1"/>
-    <col min="67" max="16384" width="9.1796875" style="3"/>
+    <col min="59" max="67" width="2.453125" style="3" customWidth="1"/>
+    <col min="68" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:67" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>64</v>
@@ -998,19 +1008,19 @@
       <c r="E1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38" t="s">
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
       <c r="O1" s="2" t="s">
         <v>67</v>
       </c>
@@ -1047,32 +1057,32 @@
       <c r="Z1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AA1" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38" t="s">
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="37" t="s">
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" s="37"/>
+      <c r="AF1" s="40"/>
       <c r="AG1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" s="38" t="s">
+      <c r="AH1" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" s="38"/>
+      <c r="AI1" s="41"/>
       <c r="AJ1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" s="38" t="s">
+      <c r="AK1" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="38"/>
+      <c r="AL1" s="41"/>
       <c r="AM1" s="2" t="s">
         <v>86</v>
       </c>
@@ -1103,10 +1113,10 @@
       <c r="AV1" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="AW1" s="36" t="s">
+      <c r="AW1" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="AX1" s="36"/>
+      <c r="AX1" s="39"/>
       <c r="AY1" s="27" t="s">
         <v>99</v>
       </c>
@@ -1125,10 +1135,10 @@
       <c r="BD1" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="BE1" s="36" t="s">
+      <c r="BE1" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="BF1" s="36"/>
+      <c r="BF1" s="39"/>
       <c r="BG1" s="27" t="s">
         <v>107</v>
       </c>
@@ -1141,16 +1151,21 @@
       <c r="BJ1" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="BK1" s="39" t="s">
+      <c r="BK1" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="BL1" s="39"/>
+      <c r="BL1" s="38"/>
       <c r="BM1" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="BN1" s="27"/>
+      <c r="BN1" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="BO1" s="27" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="2" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
@@ -1334,21 +1349,26 @@
       <c r="BI2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ2" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK2" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL2" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM2" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN2" s="26"/>
+      <c r="BJ2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL2" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM2" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN2" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO2" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="3" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1532,21 +1552,26 @@
       <c r="BI3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ3" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK3" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL3" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM3" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN3" s="26"/>
+      <c r="BJ3" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK3" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL3" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM3" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN3" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO3" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="4" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
@@ -1730,21 +1755,26 @@
       <c r="BI4" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ4" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK4" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL4" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM4" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN4" s="26"/>
+      <c r="BJ4" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK4" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL4" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM4" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO4" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="5" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>3</v>
       </c>
@@ -1928,21 +1958,26 @@
       <c r="BI5" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ5" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK5" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL5" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM5" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN5" s="26"/>
+      <c r="BJ5" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK5" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL5" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM5" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN5" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO5" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>4</v>
       </c>
@@ -2126,21 +2161,26 @@
       <c r="BI6" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ6" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK6" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL6" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM6" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN6" s="26"/>
+      <c r="BJ6" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK6" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL6" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM6" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN6" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO6" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>5</v>
       </c>
@@ -2324,21 +2364,26 @@
       <c r="BI7" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ7" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK7" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL7" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM7" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN7" s="26"/>
+      <c r="BJ7" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK7" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO7" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>6</v>
       </c>
@@ -2522,21 +2567,26 @@
       <c r="BI8" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ8" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK8" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL8" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM8" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN8" s="26"/>
+      <c r="BJ8" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK8" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL8" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM8" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO8" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>7</v>
       </c>
@@ -2720,21 +2770,26 @@
       <c r="BI9" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ9" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK9" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL9" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM9" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN9" s="26"/>
+      <c r="BJ9" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK9" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL9" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM9" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN9" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO9" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="10" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>8</v>
       </c>
@@ -2918,21 +2973,26 @@
       <c r="BI10" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ10" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK10" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL10" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM10" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN10" s="26"/>
+      <c r="BJ10" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK10" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL10" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM10" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN10" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO10" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="11" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>9</v>
       </c>
@@ -3116,21 +3176,26 @@
       <c r="BI11" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ11" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK11" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL11" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM11" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN11" s="26"/>
+      <c r="BJ11" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK11" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN11" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO11" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="12" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>10</v>
       </c>
@@ -3314,21 +3379,26 @@
       <c r="BI12" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ12" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK12" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL12" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM12" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN12" s="26"/>
+      <c r="BJ12" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK12" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL12" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM12" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO12" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="13" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>11</v>
       </c>
@@ -3512,21 +3582,26 @@
       <c r="BI13" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ13" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK13" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL13" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM13" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN13" s="26"/>
+      <c r="BJ13" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK13" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL13" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM13" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN13" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO13" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="14" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>12</v>
       </c>
@@ -3710,21 +3785,26 @@
       <c r="BI14" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ14" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK14" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL14" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM14" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN14" s="26"/>
+      <c r="BJ14" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK14" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL14" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM14" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO14" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="15" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>13</v>
       </c>
@@ -3908,21 +3988,26 @@
       <c r="BI15" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ15" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK15" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL15" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM15" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN15" s="26"/>
+      <c r="BJ15" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK15" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL15" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM15" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO15" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="16" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>14</v>
       </c>
@@ -4106,21 +4191,26 @@
       <c r="BI16" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ16" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK16" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL16" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM16" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN16" s="26"/>
+      <c r="BJ16" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK16" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL16" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM16" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN16" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO16" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="17" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>15</v>
       </c>
@@ -4304,21 +4394,26 @@
       <c r="BI17" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ17" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK17" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL17" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM17" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN17" s="26"/>
+      <c r="BJ17" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK17" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL17" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM17" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN17" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO17" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="18" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>16</v>
       </c>
@@ -4502,21 +4597,26 @@
       <c r="BI18" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ18" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK18" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL18" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM18" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN18" s="26"/>
+      <c r="BJ18" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK18" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL18" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM18" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN18" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO18" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="19" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>17</v>
       </c>
@@ -4700,21 +4800,26 @@
       <c r="BI19" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ19" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK19" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL19" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM19" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN19" s="26"/>
+      <c r="BJ19" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK19" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL19" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM19" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN19" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO19" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="20" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>18</v>
       </c>
@@ -4898,21 +5003,26 @@
       <c r="BI20" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ20" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK20" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL20" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM20" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN20" s="26"/>
+      <c r="BJ20" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK20" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL20" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM20" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN20" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO20" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="21" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>19</v>
       </c>
@@ -5096,21 +5206,26 @@
       <c r="BI21" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ21" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK21" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL21" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM21" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN21" s="26"/>
+      <c r="BJ21" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK21" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL21" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM21" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN21" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO21" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="22" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>20</v>
       </c>
@@ -5294,21 +5409,26 @@
       <c r="BI22" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ22" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK22" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL22" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM22" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN22" s="26"/>
+      <c r="BJ22" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK22" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL22" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM22" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN22" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO22" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="23" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>21</v>
       </c>
@@ -5492,21 +5612,26 @@
       <c r="BI23" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ23" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK23" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL23" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM23" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN23" s="26"/>
+      <c r="BJ23" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK23" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL23" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM23" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN23" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO23" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="24" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>22</v>
       </c>
@@ -5690,21 +5815,26 @@
       <c r="BI24" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ24" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK24" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL24" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM24" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN24" s="26"/>
+      <c r="BJ24" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK24" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL24" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM24" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN24" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO24" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="25" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>23</v>
       </c>
@@ -5888,21 +6018,26 @@
       <c r="BI25" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ25" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK25" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL25" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM25" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN25" s="26"/>
+      <c r="BJ25" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK25" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL25" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM25" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN25" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO25" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="26" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>24</v>
       </c>
@@ -6086,21 +6221,26 @@
       <c r="BI26" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ26" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK26" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL26" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM26" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN26" s="26"/>
+      <c r="BJ26" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK26" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL26" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM26" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN26" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO26" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="27" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>25</v>
       </c>
@@ -6284,21 +6424,26 @@
       <c r="BI27" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ27" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK27" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL27" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM27" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN27" s="26"/>
+      <c r="BJ27" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK27" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL27" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM27" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN27" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO27" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="28" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
         <v>26</v>
       </c>
@@ -6482,21 +6627,26 @@
       <c r="BI28" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ28" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK28" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL28" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM28" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN28" s="26"/>
+      <c r="BJ28" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK28" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL28" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM28" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN28" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO28" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="29" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
         <v>27</v>
       </c>
@@ -6680,21 +6830,26 @@
       <c r="BI29" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ29" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK29" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL29" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM29" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN29" s="26"/>
+      <c r="BJ29" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK29" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL29" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM29" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN29" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO29" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="30" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>28</v>
       </c>
@@ -6878,21 +7033,26 @@
       <c r="BI30" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ30" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK30" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL30" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM30" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN30" s="26"/>
+      <c r="BJ30" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK30" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL30" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM30" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN30" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO30" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="31" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
@@ -7076,21 +7236,26 @@
       <c r="BI31" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ31" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK31" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL31" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM31" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN31" s="26"/>
+      <c r="BJ31" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK31" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL31" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM31" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN31" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO31" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="32" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>30</v>
       </c>
@@ -7274,21 +7439,26 @@
       <c r="BI32" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ32" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK32" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL32" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM32" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN32" s="26"/>
+      <c r="BJ32" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK32" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL32" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM32" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN32" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO32" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="33" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>31</v>
       </c>
@@ -7472,21 +7642,26 @@
       <c r="BI33" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ33" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK33" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL33" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM33" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN33" s="26"/>
+      <c r="BJ33" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK33" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL33" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM33" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN33" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO33" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="34" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>32</v>
       </c>
@@ -7670,21 +7845,26 @@
       <c r="BI34" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ34" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK34" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL34" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM34" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN34" s="26"/>
+      <c r="BJ34" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK34" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL34" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM34" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN34" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO34" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="35" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>33</v>
       </c>
@@ -7868,21 +8048,26 @@
       <c r="BI35" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ35" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK35" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL35" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM35" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN35" s="26"/>
+      <c r="BJ35" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK35" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL35" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM35" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN35" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO35" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="36" spans="1:66" s="35" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:67" s="35" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
         <v>34</v>
       </c>
@@ -8066,21 +8251,26 @@
       <c r="BI36" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ36" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK36" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL36" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM36" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN36" s="26"/>
+      <c r="BJ36" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK36" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL36" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM36" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN36" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO36" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="37" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>35</v>
       </c>
@@ -8264,21 +8454,26 @@
       <c r="BI37" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ37" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK37" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL37" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM37" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN37" s="26"/>
+      <c r="BJ37" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK37" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL37" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM37" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN37" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO37" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="38" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
         <v>36</v>
       </c>
@@ -8462,21 +8657,26 @@
       <c r="BI38" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ38" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK38" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL38" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM38" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN38" s="26"/>
+      <c r="BJ38" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK38" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL38" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM38" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN38" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO38" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="39" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
         <v>37</v>
       </c>
@@ -8660,21 +8860,26 @@
       <c r="BI39" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ39" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK39" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL39" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM39" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN39" s="26"/>
+      <c r="BJ39" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK39" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL39" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM39" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN39" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO39" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="40" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
         <v>38</v>
       </c>
@@ -8858,21 +9063,26 @@
       <c r="BI40" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ40" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK40" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL40" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM40" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN40" s="26"/>
+      <c r="BJ40" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK40" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL40" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM40" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN40" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO40" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="41" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
         <v>39</v>
       </c>
@@ -9056,21 +9266,26 @@
       <c r="BI41" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ41" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK41" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL41" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM41" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN41" s="26"/>
+      <c r="BJ41" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK41" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL41" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM41" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN41" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO41" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="42" spans="1:66" s="35" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:67" s="35" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
         <v>40</v>
       </c>
@@ -9254,21 +9469,26 @@
       <c r="BI42" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ42" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK42" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL42" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM42" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN42" s="26"/>
+      <c r="BJ42" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK42" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL42" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM42" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN42" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO42" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="43" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
         <v>41</v>
       </c>
@@ -9452,21 +9672,26 @@
       <c r="BI43" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ43" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK43" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL43" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM43" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN43" s="26"/>
+      <c r="BJ43" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK43" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL43" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM43" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN43" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO43" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="44" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="25" t="s">
         <v>42</v>
       </c>
@@ -9650,21 +9875,26 @@
       <c r="BI44" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ44" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK44" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL44" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM44" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="BN44" s="26"/>
+      <c r="BJ44" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="BK44" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL44" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM44" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="BN44" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO44" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="45" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>43</v>
       </c>
@@ -9848,21 +10078,26 @@
       <c r="BI45" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ45" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK45" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL45" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM45" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN45" s="26"/>
+      <c r="BJ45" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK45" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL45" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM45" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN45" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO45" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="46" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="25" t="s">
         <v>44</v>
       </c>
@@ -10046,21 +10281,26 @@
       <c r="BI46" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ46" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK46" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL46" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM46" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN46" s="26"/>
+      <c r="BJ46" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK46" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL46" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM46" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN46" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO46" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="47" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="25" t="s">
         <v>45</v>
       </c>
@@ -10244,21 +10484,26 @@
       <c r="BI47" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ47" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK47" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL47" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM47" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN47" s="26"/>
+      <c r="BJ47" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK47" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL47" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM47" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN47" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO47" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="48" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="25" t="s">
         <v>46</v>
       </c>
@@ -10442,21 +10687,26 @@
       <c r="BI48" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ48" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK48" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL48" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM48" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN48" s="26"/>
+      <c r="BJ48" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK48" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL48" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM48" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN48" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO48" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="49" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="25" t="s">
         <v>47</v>
       </c>
@@ -10640,21 +10890,26 @@
       <c r="BI49" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ49" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK49" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL49" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM49" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN49" s="26"/>
+      <c r="BJ49" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK49" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL49" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM49" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN49" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO49" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="50" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
         <v>48</v>
       </c>
@@ -10838,21 +11093,26 @@
       <c r="BI50" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ50" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK50" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL50" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM50" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN50" s="26"/>
+      <c r="BJ50" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK50" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL50" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM50" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN50" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO50" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="51" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
         <v>49</v>
       </c>
@@ -11036,21 +11296,26 @@
       <c r="BI51" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ51" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK51" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL51" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM51" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN51" s="26"/>
+      <c r="BJ51" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK51" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL51" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM51" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN51" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO51" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="52" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
         <v>50</v>
       </c>
@@ -11234,21 +11499,26 @@
       <c r="BI52" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ52" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK52" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL52" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="BM52" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN52" s="26"/>
+      <c r="BJ52" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK52" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL52" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="BM52" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN52" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO52" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="53" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
         <v>52</v>
       </c>
@@ -11432,21 +11702,26 @@
       <c r="BI53" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ53" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK53" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL53" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM53" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN53" s="26"/>
+      <c r="BJ53" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK53" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL53" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM53" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN53" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO53" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="54" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="25" t="s">
         <v>51</v>
       </c>
@@ -11630,21 +11905,26 @@
       <c r="BI54" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ54" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK54" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL54" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM54" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN54" s="26"/>
+      <c r="BJ54" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK54" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL54" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM54" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN54" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO54" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="55" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="25" t="s">
         <v>53</v>
       </c>
@@ -11828,21 +12108,26 @@
       <c r="BI55" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ55" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK55" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL55" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM55" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN55" s="26"/>
+      <c r="BJ55" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK55" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL55" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM55" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN55" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO55" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="56" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="25" t="s">
         <v>54</v>
       </c>
@@ -12026,21 +12311,26 @@
       <c r="BI56" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ56" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK56" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL56" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM56" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN56" s="26"/>
+      <c r="BJ56" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK56" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL56" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM56" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN56" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO56" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="57" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="25" t="s">
         <v>55</v>
       </c>
@@ -12224,21 +12514,26 @@
       <c r="BI57" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ57" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK57" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL57" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM57" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN57" s="26"/>
+      <c r="BJ57" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK57" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL57" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM57" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN57" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="BO57" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="58" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="25" t="s">
         <v>56</v>
       </c>
@@ -12422,21 +12717,26 @@
       <c r="BI58" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ58" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK58" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL58" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM58" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN58" s="26"/>
+      <c r="BJ58" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK58" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL58" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM58" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN58" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO58" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="59" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
@@ -12620,21 +12920,26 @@
       <c r="BI59" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ59" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK59" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL59" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM59" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN59" s="26"/>
+      <c r="BJ59" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK59" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL59" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM59" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN59" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO59" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="60" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="25" t="s">
         <v>58</v>
       </c>
@@ -12818,21 +13123,26 @@
       <c r="BI60" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ60" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK60" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL60" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM60" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN60" s="26"/>
+      <c r="BJ60" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK60" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL60" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM60" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN60" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO60" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="61" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
         <v>59</v>
       </c>
@@ -13016,21 +13326,26 @@
       <c r="BI61" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ61" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK61" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL61" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM61" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN61" s="26"/>
+      <c r="BJ61" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK61" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL61" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM61" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN61" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO61" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="62" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
         <v>60</v>
       </c>
@@ -13214,21 +13529,26 @@
       <c r="BI62" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ62" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK62" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL62" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM62" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN62" s="26"/>
+      <c r="BJ62" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK62" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL62" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM62" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN62" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO62" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="63" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>61</v>
       </c>
@@ -13412,21 +13732,26 @@
       <c r="BI63" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ63" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK63" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL63" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM63" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN63" s="26"/>
+      <c r="BJ63" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK63" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL63" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM63" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN63" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO63" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="64" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="25" t="s">
         <v>62</v>
       </c>
@@ -13473,7 +13798,7 @@
         <v>90</v>
       </c>
       <c r="P64" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q64" s="9" t="s">
         <v>91</v>
@@ -13610,21 +13935,26 @@
       <c r="BI64" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ64" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK64" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="BL64" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM64" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN64" s="26"/>
+      <c r="BJ64" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK64" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="BL64" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM64" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN64" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO64" s="26" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="65" spans="1:66" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:67" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="25" t="s">
         <v>63</v>
       </c>
@@ -13808,19 +14138,24 @@
       <c r="BI65" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BJ65" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BK65" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL65" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM65" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="BN65" s="26"/>
+      <c r="BJ65" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK65" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="BL65" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM65" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN65" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="BO65" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>